<commit_message>
scénario et phrases use case
</commit_message>
<xml_diff>
--- a/Documentation/Scénario.xlsx
+++ b/Documentation/Scénario.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Inscription" sheetId="1" r:id="rId1"/>
     <sheet name="Connexion" sheetId="2" r:id="rId2"/>
+    <sheet name="Modifier" sheetId="3" r:id="rId3"/>
+    <sheet name="Poster" sheetId="4" r:id="rId4"/>
+    <sheet name="Supprimer" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Cas</t>
   </si>
@@ -127,6 +130,18 @@
   </si>
   <si>
     <t>Renvoi sur la page "Register"</t>
+  </si>
+  <si>
+    <t>Connexion</t>
+  </si>
+  <si>
+    <t>Poster</t>
+  </si>
+  <si>
+    <t>Modifier</t>
+  </si>
+  <si>
+    <t>Supprimer</t>
   </si>
 </sst>
 </file>
@@ -535,7 +550,7 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +682,7 @@
   <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B2" sqref="B2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -690,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -780,4 +795,140 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>